<commit_message>
MàJ Mockup + Ajout Modèles & Web Services
</commit_message>
<xml_diff>
--- a/GestiBank - Suivi du projet.xlsx
+++ b/GestiBank - Suivi du projet.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Adrien/Documents/Adrien/Travail/Global Knowledge/GestiBank/GestiBank-Divers/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{62CF2D9E-C12D-D84E-8066-C50E186403EB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1245" windowWidth="28800" windowHeight="15540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan d'actions" sheetId="2" r:id="rId1"/>
@@ -15,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="142">
   <si>
     <t>Status</t>
   </si>
@@ -90,18 +96,9 @@
     <t>Créer un dépôt GitHub pour le projet</t>
   </si>
   <si>
-    <t>Créer le plan du site de l'application</t>
-  </si>
-  <si>
-    <t>Créer la maquette du site de l'application</t>
-  </si>
-  <si>
     <t>MàJ Routing</t>
   </si>
   <si>
-    <t>MàJ Maquette du site</t>
-  </si>
-  <si>
     <t>Routing Module Admin</t>
   </si>
   <si>
@@ -109,10 +106,6 @@
   </si>
   <si>
     <t>Routing Module Conseiller</t>
-  </si>
-  <si>
-    <t>- Vérifier la maquette par rapport au cahier des charge
-- Mettre à jour la maquette par rapport au routing de l'application</t>
   </si>
   <si>
     <t>Mettre en place le routing général de l'application</t>
@@ -417,12 +410,52 @@
   </si>
   <si>
     <t>Partie fonctionnelles des composants (hors DashBoard)</t>
+  </si>
+  <si>
+    <t>Vérification de la maquette du site</t>
+  </si>
+  <si>
+    <t>Vérification Maquette du site</t>
+  </si>
+  <si>
+    <t>Créer le plan du site</t>
+  </si>
+  <si>
+    <t>Créer la maquette du site</t>
+  </si>
+  <si>
+    <t>BackEnd</t>
+  </si>
+  <si>
+    <t>Architecture du BackEnd</t>
+  </si>
+  <si>
+    <t>3/4</t>
+  </si>
+  <si>
+    <t>FrontEnd
+BackEnd</t>
+  </si>
+  <si>
+    <t>Mettre en place les tests des Web Services via SoapUI</t>
+  </si>
+  <si>
+    <t>Test Web Services</t>
+  </si>
+  <si>
+    <t>Créer l'architecture du BackEnd</t>
+  </si>
+  <si>
+    <t>Essai Web Services</t>
+  </si>
+  <si>
+    <t>Tester la consommation d'un web service (BackEnd) par l'application (FrontEnd)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -602,22 +635,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -629,13 +653,22 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -698,7 +731,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -731,9 +764,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -766,6 +816,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -941,401 +1008,411 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="4" max="4" width="82.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="82.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="4"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
+        <v>0</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="12"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="10">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="11"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="11"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="11"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="12"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="10">
+        <v>2</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="11"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="12"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10">
+        <v>3</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="11"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>4</v>
+      </c>
+      <c r="B19" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10" t="s">
+      <c r="C19" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="11"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="11"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="12"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="10">
+        <v>5</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="11"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="11"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="12"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="10">
+        <v>6</v>
+      </c>
+      <c r="B27" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="10"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="19">
-        <v>0</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
-        <v>1</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="19">
-        <v>2</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19">
-        <v>3</v>
-      </c>
-      <c r="B16" s="16" t="s">
+      <c r="C27" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="11"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="11"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="11"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="11"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="12"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="10">
+        <v>7</v>
+      </c>
+      <c r="B33" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
-        <v>4</v>
-      </c>
-      <c r="B19" s="16" t="s">
+      <c r="C33" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="19">
-        <v>5</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="19">
-        <v>6</v>
-      </c>
-      <c r="B27" s="16" t="s">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="12"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="10">
+        <v>8</v>
+      </c>
+      <c r="B35" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="D31" s="9" t="s">
+      <c r="C35" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D35" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="19">
-        <v>7</v>
-      </c>
-      <c r="B33" s="16" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="12"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D36" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="19">
-        <v>8</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B16:B18"/>
     <mergeCell ref="A19:A22"/>
     <mergeCell ref="B19:B22"/>
     <mergeCell ref="A23:A26"/>
@@ -1346,16 +1423,6 @@
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="A27:A32"/>
     <mergeCell ref="B27:B32"/>
-    <mergeCell ref="A7:A12"/>
-    <mergeCell ref="B7:B12"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1363,49 +1430,49 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" customWidth="1"/>
+    <col min="4" max="4" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.95" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="14" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>21</v>
@@ -1416,14 +1483,14 @@
       <c r="D4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-    </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>3</v>
@@ -1447,18 +1514,18 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>9</v>
@@ -1473,9 +1540,9 @@
         <v>43270</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>4</v>
@@ -1484,7 +1551,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>24</v>
+        <v>131</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>18</v>
@@ -1499,9 +1566,9 @@
         <v>43270</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>4</v>
@@ -1510,7 +1577,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>25</v>
+        <v>132</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>5</v>
@@ -1525,9 +1592,9 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>6</v>
@@ -1536,7 +1603,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>5</v>
@@ -1551,18 +1618,18 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>10</v>
@@ -1577,18 +1644,18 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>10</v>
@@ -1603,18 +1670,18 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>9</v>
@@ -1629,18 +1696,18 @@
         <v>43272</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>9</v>
@@ -1655,18 +1722,18 @@
         <v>43272</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>5</v>
@@ -1681,18 +1748,18 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>5</v>
@@ -1707,18 +1774,18 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>8</v>
@@ -1733,9 +1800,9 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>6</v>
@@ -1744,7 +1811,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>8</v>
@@ -1759,9 +1826,9 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>6</v>
@@ -1770,7 +1837,7 @@
         <v>11</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>8</v>
@@ -1785,114 +1852,122 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>26</v>
+        <v>130</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>12</v>
+      <c r="F19" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="G19" s="3">
         <v>43272</v>
       </c>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H19" s="3">
+        <v>43280</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="7" t="s">
-        <v>12</v>
+      <c r="F20" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="G20" s="3">
         <v>43272</v>
       </c>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="H20" s="3">
+        <v>43280</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="7" t="s">
-        <v>12</v>
+      <c r="F21" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="G21" s="3">
         <v>43272</v>
       </c>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H21" s="3">
+        <v>43280</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="7" t="s">
-        <v>12</v>
+      <c r="F22" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="G22" s="3">
         <v>43276</v>
       </c>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="H22" s="3">
+        <v>43280</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>18</v>
@@ -1905,45 +1980,183 @@
       </c>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="3">
+        <v>43281</v>
+      </c>
+      <c r="H24" s="3">
+        <v>43282</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="3">
+        <v>43281</v>
+      </c>
+      <c r="H25" s="3">
+        <v>43282</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="3">
+        <v>43281</v>
+      </c>
+      <c r="H26" s="3">
+        <v>43282</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
MaJ Suivi des actions
</commit_message>
<xml_diff>
--- a/GestiBank - Suivi du projet.xlsx
+++ b/GestiBank - Suivi du projet.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Adrien/Documents/Adrien/Travail/Global Knowledge/GestiBank/GestiBank-Divers/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BE5990AB-D9A4-B34D-AF40-A720FC58E8E9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16395"/>
   </bookViews>
   <sheets>
     <sheet name="Plan d'actions" sheetId="2" r:id="rId1"/>
@@ -21,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="178">
   <si>
     <t>Status</t>
   </si>
@@ -243,9 +237,6 @@
     <t>1.6</t>
   </si>
   <si>
-    <t>Réaliser la description fonctionnelle des Web Services</t>
-  </si>
-  <si>
     <t>Routing</t>
   </si>
   <si>
@@ -534,12 +525,43 @@
   </si>
   <si>
     <t>BackEnd - Couche Services</t>
+  </si>
+  <si>
+    <t>Modeles et Services</t>
+  </si>
+  <si>
+    <t>Préparer le fichier de suivi :
+- modeles
+- couche "DAO"
+- couche "Services"
+- couche "Web Services"</t>
+  </si>
+  <si>
+    <t>1.4/1.5/1.6</t>
+  </si>
+  <si>
+    <t>Webs Services</t>
+  </si>
+  <si>
+    <t>Implémentation des Webs Services</t>
+  </si>
+  <si>
+    <t>Implémenter le Web Service associé à l'espace Public</t>
+  </si>
+  <si>
+    <t>Implémenter le Web Service associé à l'espace Admin</t>
+  </si>
+  <si>
+    <t>Implémenter le Web Service associé à l'espace Conseiller</t>
+  </si>
+  <si>
+    <t>Implémenter le Web Service associé à l'espace Client</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -711,19 +733,19 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -801,7 +823,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -834,26 +856,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -886,23 +891,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1078,38 +1066,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="82.5" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="82.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18.95" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B1" s="4"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="15"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3" s="13"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>0</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -1119,19 +1107,19 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
-      <c r="B5" s="13"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="7" t="s">
         <v>59</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="13"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="7" t="s">
         <v>60</v>
       </c>
@@ -1139,11 +1127,11 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>1</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="15" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -1153,9 +1141,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
-      <c r="B8" s="13"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="7" t="s">
         <v>68</v>
       </c>
@@ -1163,9 +1151,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
-      <c r="B9" s="13"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="7" t="s">
         <v>69</v>
       </c>
@@ -1173,9 +1161,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
-      <c r="B10" s="13"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="7" t="s">
         <v>70</v>
       </c>
@@ -1183,9 +1171,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
-      <c r="B11" s="13"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="7" t="s">
         <v>71</v>
       </c>
@@ -1193,9 +1181,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
-      <c r="B12" s="13"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="7" t="s">
         <v>72</v>
       </c>
@@ -1203,316 +1191,318 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>2</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>121</v>
+      <c r="B13" s="15" t="s">
+        <v>120</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="7" t="s">
+      <c r="D14" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="7" t="s">
-        <v>77</v>
-      </c>
       <c r="D15" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>3</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>120</v>
+      <c r="B16" s="15" t="s">
+        <v>119</v>
       </c>
       <c r="C16" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="7" t="s">
-        <v>83</v>
-      </c>
       <c r="D17" s="8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>4</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="15" t="s">
         <v>38</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D19" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
         <v>5</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="15" t="s">
         <v>39</v>
       </c>
       <c r="C20" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="7" t="s">
+      <c r="D21" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="7" t="s">
-        <v>89</v>
-      </c>
       <c r="D22" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
-      <c r="B24" s="13"/>
+      <c r="B24" s="15"/>
       <c r="C24" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
         <v>6</v>
       </c>
-      <c r="B25" s="13" t="s">
-        <v>122</v>
+      <c r="B25" s="15" t="s">
+        <v>121</v>
       </c>
       <c r="C25" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D26" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="8" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="14"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="14"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="7" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D28" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="7" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="14"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="7" t="s">
-        <v>94</v>
-      </c>
       <c r="D29" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <v>7</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="C30" s="7" t="s">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D31" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="7" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="14"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D31" s="8" t="s">
+      <c r="D32" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="14"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="14"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="7" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="D33" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="14"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="7" t="s">
-        <v>133</v>
-      </c>
       <c r="D34" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="14">
         <v>8</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="15" t="s">
         <v>40</v>
       </c>
       <c r="C35" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D36" s="8" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="14"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D36" s="8" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="14"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="14">
         <v>9</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="15" t="s">
         <v>42</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="14"/>
-      <c r="B39" s="13"/>
+      <c r="B39" s="15"/>
       <c r="C39" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D39" s="8" t="s">
         <v>139</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="A7:A12"/>
-    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="B30:B34"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:B37"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A18:A19"/>
@@ -1521,14 +1511,12 @@
     <mergeCell ref="B20:B24"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A30:A34"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="B7:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1536,27 +1524,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="26.83203125" customWidth="1"/>
-    <col min="4" max="4" width="29.1640625" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18.95" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>37</v>
       </c>
@@ -1576,7 +1564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>45</v>
       </c>
@@ -1594,7 +1582,7 @@
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>59</v>
       </c>
@@ -1620,7 +1608,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>60</v>
       </c>
@@ -1646,7 +1634,7 @@
         <v>43270</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>67</v>
       </c>
@@ -1657,7 +1645,7 @@
         <v>16</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>17</v>
@@ -1672,7 +1660,7 @@
         <v>43270</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>68</v>
       </c>
@@ -1683,7 +1671,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>5</v>
@@ -1698,9 +1686,9 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>6</v>
@@ -1724,9 +1712,9 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>6</v>
@@ -1752,7 +1740,7 @@
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>6</v>
@@ -1776,9 +1764,9 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>6</v>
@@ -1804,7 +1792,7 @@
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>6</v>
@@ -1828,9 +1816,9 @@
         <v>43272</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>6</v>
@@ -1856,7 +1844,7 @@
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>6</v>
@@ -1880,9 +1868,9 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>6</v>
@@ -1908,7 +1896,7 @@
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>6</v>
@@ -1932,9 +1920,9 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>6</v>
@@ -1943,7 +1931,7 @@
         <v>11</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>8</v>
@@ -1958,7 +1946,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>68</v>
       </c>
@@ -1966,10 +1954,10 @@
         <v>4</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>119</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>8</v>
@@ -1984,9 +1972,9 @@
         <v>43280</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>6</v>
@@ -2010,7 +1998,7 @@
         <v>43280</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>71</v>
       </c>
@@ -2021,7 +2009,7 @@
         <v>33</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>9</v>
@@ -2036,7 +2024,7 @@
         <v>43280</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>69</v>
       </c>
@@ -2044,10 +2032,10 @@
         <v>4</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>17</v>
@@ -2062,18 +2050,18 @@
         <v>43280</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>108</v>
-      </c>
       <c r="D23" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>5</v>
@@ -2088,18 +2076,18 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>146</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>5</v>
@@ -2116,16 +2104,16 @@
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>5</v>
@@ -2140,18 +2128,18 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>5</v>
@@ -2166,7 +2154,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>72</v>
       </c>
@@ -2177,10 +2165,10 @@
         <v>34</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>12</v>
@@ -2192,18 +2180,18 @@
         <v>43285</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>5</v>
@@ -2218,9 +2206,9 @@
         <v>43284</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>6</v>
@@ -2229,7 +2217,7 @@
         <v>38</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>8</v>
@@ -2244,68 +2232,72 @@
         <v>43285</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B30" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="E30" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E30" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="12" t="s">
-        <v>150</v>
+      <c r="F30" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="G30" s="3">
         <v>43285</v>
       </c>
-      <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A31" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>4</v>
+      <c r="H30" s="3">
+        <v>43285</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>154</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>73</v>
+        <v>163</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>164</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>150</v>
+        <v>5</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="G31" s="3">
-        <v>43286</v>
-      </c>
-      <c r="H31" s="3"/>
-    </row>
-    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+        <v>43287</v>
+      </c>
+      <c r="H31" s="3">
+        <v>43289</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C32" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="B32" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>164</v>
-      </c>
       <c r="D32" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="E32" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E32" s="10" t="s">
         <v>5</v>
       </c>
       <c r="F32" s="6" t="s">
@@ -2318,20 +2310,20 @@
         <v>43289</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B33" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="C33" s="11" t="s">
+      <c r="B33" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C33" s="10" t="s">
         <v>157</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="10" t="s">
         <v>5</v>
       </c>
       <c r="F33" s="6" t="s">
@@ -2344,20 +2336,20 @@
         <v>43289</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="E34" s="11" t="s">
+    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E34" s="10" t="s">
         <v>5</v>
       </c>
       <c r="F34" s="6" t="s">
@@ -2370,95 +2362,179 @@
         <v>43289</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A35" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="E35" s="11" t="s">
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="E35" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F35" s="6" t="s">
-        <v>12</v>
+      <c r="F35" s="11" t="s">
+        <v>149</v>
       </c>
       <c r="G35" s="3">
         <v>43287</v>
       </c>
-      <c r="H35" s="3">
-        <v>43289</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="E36" s="11" t="s">
+      <c r="H35" s="3"/>
+    </row>
+    <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="G36" s="3">
+        <v>43291</v>
+      </c>
+      <c r="H36" s="3"/>
+    </row>
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="G37" s="3">
+        <v>43291</v>
+      </c>
+      <c r="H37" s="3"/>
+    </row>
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="G38" s="3">
+        <v>43291</v>
+      </c>
+      <c r="H38" s="3"/>
+    </row>
+    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="E39" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F36" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="G36" s="3">
-        <v>43287</v>
-      </c>
-      <c r="H36" s="3"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="7"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="7"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="7"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
+      <c r="F39" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="G39" s="3">
+        <v>43291</v>
+      </c>
+      <c r="H39" s="3"/>
+    </row>
+    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="G40" s="3">
+        <v>43291</v>
+      </c>
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="7"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2471,7 +2547,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A26 A36" numberStoredAsText="1"/>
+    <ignoredError sqref="A26 A35 A37 A38:A40" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>